<commit_message>
Continue extracting the CE_b tables.
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/Std140_CE_b_Output.xlsx
+++ b/input/Test/0.0.0/Std140_CE_b_Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B481584-8FF0-4AB5-801E-4B50AECFB8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8941D7-DBBD-4CE8-8BAC-636F9DE22C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24825" yWindow="1830" windowWidth="30675" windowHeight="17970" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
+    <workbookView xWindow="11625" yWindow="1515" windowWidth="25725" windowHeight="18000" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
     <t>Sens+Lat</t>
   </si>
   <si>
-    <t>TEST 0.0.0</t>
+    <t>TEST 0.0.0 received September 1, 2024</t>
   </si>
 </sst>
 </file>
@@ -1533,7 +1533,7 @@
   </sheetPr>
   <dimension ref="A1:AO214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finish up CE_b excel processing and cleansing
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/Std140_CE_b_Output.xlsx
+++ b/input/Test/0.0.0/Std140_CE_b_Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8941D7-DBBD-4CE8-8BAC-636F9DE22C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F604A6-722E-4878-8258-7668F01E2E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11625" yWindow="1515" windowWidth="25725" windowHeight="18000" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
+    <workbookView xWindow="3525" yWindow="165" windowWidth="39120" windowHeight="17865" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -1533,8 +1533,8 @@
   </sheetPr>
   <dimension ref="A1:AO214"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P76" sqref="P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3451,7 +3451,7 @@
       <c r="N74" s="22"/>
       <c r="O74" s="22"/>
       <c r="P74" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q74" s="23">
         <f t="shared" si="2"/>
@@ -6473,7 +6473,7 @@
         <v>101593.51037732697</v>
       </c>
       <c r="P101" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q101" s="25">
         <f t="shared" si="24"/>

</xml_diff>

<commit_message>
Update the test program spreadsheet
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/Std140_CE_b_Output.xlsx
+++ b/input/Test/0.0.0/Std140_CE_b_Output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B39EEE7-DB40-4268-8DB8-BBD24CC02274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E502147-8204-4C66-A756-B8CE261B1CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="4110" windowWidth="40575" windowHeight="15465" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
+    <workbookView xWindow="3660" yWindow="810" windowWidth="33600" windowHeight="20790" xr2:uid="{6C5182BB-48B8-4F6B-8426-D0FB240A2181}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="170">
   <si>
     <t>E300OUT2.XLS, Mar 20, 2002</t>
   </si>
@@ -233,12 +233,6 @@
     <t xml:space="preserve">   A n n u a l   H o u r l y   I n t e g r a t e d   M a x i m a   C o n s u m p t i o n s   a n d   L o a d s</t>
   </si>
   <si>
-    <t xml:space="preserve">         E300 Only, Maxima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E 3 0 0   O n l y</t>
-  </si>
-  <si>
     <t>Zone</t>
   </si>
   <si>
@@ -332,75 +326,6 @@
     <t>kg/kg</t>
   </si>
   <si>
-    <t>E300</t>
-  </si>
-  <si>
-    <t>E310</t>
-  </si>
-  <si>
-    <t>E320</t>
-  </si>
-  <si>
-    <t>E330</t>
-  </si>
-  <si>
-    <t>E340</t>
-  </si>
-  <si>
-    <t>E350</t>
-  </si>
-  <si>
-    <t>E360</t>
-  </si>
-  <si>
-    <t>E400</t>
-  </si>
-  <si>
-    <t>E410</t>
-  </si>
-  <si>
-    <t>E420</t>
-  </si>
-  <si>
-    <t>E430</t>
-  </si>
-  <si>
-    <t>E440</t>
-  </si>
-  <si>
-    <t>E500</t>
-  </si>
-  <si>
-    <t>E500 May-Sep</t>
-  </si>
-  <si>
-    <t>E510</t>
-  </si>
-  <si>
-    <t>E510 May-Sep</t>
-  </si>
-  <si>
-    <t>E520</t>
-  </si>
-  <si>
-    <t>E522</t>
-  </si>
-  <si>
-    <t>E525</t>
-  </si>
-  <si>
-    <t>E530</t>
-  </si>
-  <si>
-    <t>E540</t>
-  </si>
-  <si>
-    <t>E545</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> J u n e   2 8   H o u r l y   O u t p u t   -   C a s e   E 3 0 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">             A n n u a l   H o u r l y   I n t e g r a t e d   M a x i m a   a n d   M i n i m a   -   C O P 2   a n d   Z o n e</t>
   </si>
   <si>
@@ -521,9 +446,6 @@
     <t>24</t>
   </si>
   <si>
-    <t xml:space="preserve">      C a s e   E 5 0 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Evaporator Coil Load</t>
   </si>
   <si>
@@ -539,13 +461,94 @@
     <t>June 25</t>
   </si>
   <si>
-    <t xml:space="preserve">      C a s e   E 5 3 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
-  </si>
-  <si>
     <t>system off gives 0.000</t>
   </si>
   <si>
     <t>TEST 0.0.0 received September 1, 2024</t>
+  </si>
+  <si>
+    <t>CE300</t>
+  </si>
+  <si>
+    <t>CE310</t>
+  </si>
+  <si>
+    <t>CE320</t>
+  </si>
+  <si>
+    <t>CE330</t>
+  </si>
+  <si>
+    <t>CE340</t>
+  </si>
+  <si>
+    <t>CE350</t>
+  </si>
+  <si>
+    <t>CE360</t>
+  </si>
+  <si>
+    <t>CE400</t>
+  </si>
+  <si>
+    <t>CE410</t>
+  </si>
+  <si>
+    <t>CE420</t>
+  </si>
+  <si>
+    <t>CE430</t>
+  </si>
+  <si>
+    <t>CE440</t>
+  </si>
+  <si>
+    <t>CE500</t>
+  </si>
+  <si>
+    <t>CE500 May-Sep</t>
+  </si>
+  <si>
+    <t>CE510 May-Sep</t>
+  </si>
+  <si>
+    <t>CE520</t>
+  </si>
+  <si>
+    <t>CE522</t>
+  </si>
+  <si>
+    <t>CE525</t>
+  </si>
+  <si>
+    <t>CE530</t>
+  </si>
+  <si>
+    <t>CE540</t>
+  </si>
+  <si>
+    <t>CE545</t>
+  </si>
+  <si>
+    <t>C E 3 0 0   O n l y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE500 </t>
+  </si>
+  <si>
+    <t>CE510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         CE300 Only, Maxima</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J u n e   2 8   H o u r l y   O u t p u t   -   C a s e   C E 3 0 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      C a s e   C E 5 0 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      C a s e   C E 5 3 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
   </si>
 </sst>
 </file>
@@ -1282,8 +1285,8 @@
   </sheetPr>
   <dimension ref="A1:AN130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM101" sqref="AM101:AM108"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1300,7 +1303,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1610,7 +1613,7 @@
       <c r="AB56" s="7"/>
       <c r="AC56" s="5"/>
       <c r="AD56" s="6" t="s">
-        <v>64</v>
+        <v>166</v>
       </c>
       <c r="AE56" s="6"/>
       <c r="AF56" s="6"/>
@@ -1631,7 +1634,7 @@
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="11" t="s">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="N57" s="13"/>
       <c r="P57" s="10"/>
@@ -1659,14 +1662,14 @@
       <c r="B58" s="10"/>
       <c r="I58" s="10"/>
       <c r="K58" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M58" s="10"/>
       <c r="N58" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="10"/>
@@ -1675,37 +1678,37 @@
       <c r="S58" s="7"/>
       <c r="AB58" s="15"/>
       <c r="AD58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AH58" s="7"/>
     </row>
     <row r="59" spans="1:34">
       <c r="A59" s="10"/>
       <c r="B59" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I59" s="10"/>
       <c r="K59" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M59" s="10"/>
       <c r="N59" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="10"/>
       <c r="Q59" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="S59" s="15"/>
       <c r="V59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AB59" s="15"/>
       <c r="AE59" s="15"/>
@@ -1713,118 +1716,118 @@
     </row>
     <row r="60" spans="1:34">
       <c r="A60" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="D60" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="F60" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F60" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G60" s="2" t="s">
+      <c r="I60" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="J60" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I60" s="17" t="s">
+      <c r="K60" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="L60" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M60" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="K60" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M60" s="17" t="s">
-        <v>85</v>
-      </c>
       <c r="N60" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q60" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T60" s="10"/>
       <c r="U60" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="W60" s="10"/>
       <c r="X60" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Z60" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AB60" s="15"/>
       <c r="AD60" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AE60" s="15"/>
       <c r="AF60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AH60" s="15"/>
     </row>
     <row r="61" spans="1:34">
       <c r="A61" s="11"/>
       <c r="B61" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F61" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H61" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I61" s="11"/>
       <c r="J61" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K61" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="L61" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="K61" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="L61" s="19" t="s">
-        <v>93</v>
-      </c>
       <c r="M61" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N61" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O61" s="19"/>
       <c r="P61" s="11"/>
       <c r="Q61" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R61" s="19" t="s">
         <v>57</v>
@@ -1833,7 +1836,7 @@
         <v>58</v>
       </c>
       <c r="T61" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="U61" s="19" t="s">
         <v>57</v>
@@ -1842,7 +1845,7 @@
         <v>58</v>
       </c>
       <c r="W61" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X61" s="19" t="s">
         <v>57</v>
@@ -1851,7 +1854,7 @@
         <v>58</v>
       </c>
       <c r="Z61" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AA61" s="19" t="s">
         <v>57</v>
@@ -1860,7 +1863,7 @@
         <v>58</v>
       </c>
       <c r="AC61" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AD61" s="19" t="s">
         <v>57</v>
@@ -1869,7 +1872,7 @@
         <v>58</v>
       </c>
       <c r="AF61" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AG61" s="19" t="s">
         <v>57</v>
@@ -1880,7 +1883,7 @@
     </row>
     <row r="62" spans="1:34" ht="15.75">
       <c r="A62" s="10" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="B62" s="21">
         <v>34755</v>
@@ -1923,7 +1926,7 @@
       </c>
       <c r="O62" s="22"/>
       <c r="P62" s="10" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="Q62" s="23">
         <v>11602</v>
@@ -1982,7 +1985,7 @@
     </row>
     <row r="63" spans="1:34" ht="15.75">
       <c r="A63" s="10" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="B63" s="21">
         <v>39384</v>
@@ -2021,7 +2024,7 @@
       <c r="N63" s="36"/>
       <c r="O63" s="22"/>
       <c r="P63" s="10" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="Q63" s="23">
         <v>12595</v>
@@ -2062,7 +2065,7 @@
     </row>
     <row r="64" spans="1:34" ht="15.75">
       <c r="A64" s="10" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="B64" s="21">
         <v>38792</v>
@@ -2101,7 +2104,7 @@
       <c r="N64" s="36"/>
       <c r="O64" s="22"/>
       <c r="P64" s="10" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="Q64" s="23">
         <v>12981</v>
@@ -2142,7 +2145,7 @@
     </row>
     <row r="65" spans="1:28" ht="15.75">
       <c r="A65" s="10" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="B65" s="21">
         <v>39438</v>
@@ -2181,7 +2184,7 @@
       <c r="N65" s="22"/>
       <c r="O65" s="22"/>
       <c r="P65" s="10" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="Q65" s="23">
         <v>13407</v>
@@ -2222,7 +2225,7 @@
     </row>
     <row r="66" spans="1:28" ht="15.75">
       <c r="A66" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="B66" s="21">
         <v>39265</v>
@@ -2261,7 +2264,7 @@
       <c r="N66" s="22"/>
       <c r="O66" s="22"/>
       <c r="P66" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="Q66" s="23">
         <v>13190</v>
@@ -2302,7 +2305,7 @@
     </row>
     <row r="67" spans="1:28" ht="15.75">
       <c r="A67" s="10" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="B67" s="21">
         <v>30548</v>
@@ -2341,7 +2344,7 @@
       <c r="N67" s="22"/>
       <c r="O67" s="22"/>
       <c r="P67" s="10" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="Q67" s="23">
         <v>11602</v>
@@ -2382,7 +2385,7 @@
     </row>
     <row r="68" spans="1:28" ht="15.75">
       <c r="A68" s="10" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="B68" s="21">
         <v>54016</v>
@@ -2421,7 +2424,7 @@
       <c r="N68" s="22"/>
       <c r="O68" s="22"/>
       <c r="P68" s="10" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="Q68" s="23">
         <v>12726</v>
@@ -2462,7 +2465,7 @@
     </row>
     <row r="69" spans="1:28" ht="15.75">
       <c r="A69" s="10" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="B69" s="21">
         <v>30876</v>
@@ -2501,7 +2504,7 @@
       <c r="N69" s="22"/>
       <c r="O69" s="22"/>
       <c r="P69" s="10" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="Q69" s="23">
         <v>11677</v>
@@ -2542,7 +2545,7 @@
     </row>
     <row r="70" spans="1:28" ht="15.75">
       <c r="A70" s="10" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="B70" s="21">
         <v>31699</v>
@@ -2581,7 +2584,7 @@
       <c r="N70" s="22"/>
       <c r="O70" s="22"/>
       <c r="P70" s="10" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="Q70" s="23">
         <v>11602</v>
@@ -2622,7 +2625,7 @@
     </row>
     <row r="71" spans="1:28" ht="15.75">
       <c r="A71" s="10" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="B71" s="21">
         <v>32910</v>
@@ -2661,7 +2664,7 @@
       <c r="N71" s="22"/>
       <c r="O71" s="22"/>
       <c r="P71" s="10" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="Q71" s="23">
         <v>11602</v>
@@ -2702,7 +2705,7 @@
     </row>
     <row r="72" spans="1:28" ht="15.75">
       <c r="A72" s="10" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="B72" s="21">
         <v>31811</v>
@@ -2741,7 +2744,7 @@
       <c r="N72" s="22"/>
       <c r="O72" s="22"/>
       <c r="P72" s="10" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="Q72" s="23">
         <v>11602</v>
@@ -2782,7 +2785,7 @@
     </row>
     <row r="73" spans="1:28" ht="15.75">
       <c r="A73" s="10" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="B73" s="21">
         <v>32973</v>
@@ -2821,7 +2824,7 @@
       <c r="N73" s="22"/>
       <c r="O73" s="22"/>
       <c r="P73" s="10" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="Q73" s="23">
         <v>11602</v>
@@ -2862,7 +2865,7 @@
     </row>
     <row r="74" spans="1:28" ht="15.75">
       <c r="A74" s="10" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="B74" s="21">
         <v>22822</v>
@@ -2897,7 +2900,7 @@
       <c r="N74" s="22"/>
       <c r="O74" s="22"/>
       <c r="P74" s="10" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="Q74" s="23">
         <v>10425</v>
@@ -2938,7 +2941,7 @@
     </row>
     <row r="75" spans="1:28" ht="15.75">
       <c r="A75" s="10" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="B75" s="21">
         <v>17870</v>
@@ -2977,7 +2980,7 @@
       <c r="N75" s="22"/>
       <c r="O75" s="22"/>
       <c r="P75" s="10" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="Q75" s="23">
         <v>11587</v>
@@ -3018,7 +3021,7 @@
     </row>
     <row r="76" spans="1:28" ht="15.75">
       <c r="A76" s="10" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="B76" s="21">
         <v>35970</v>
@@ -3057,7 +3060,7 @@
       <c r="N76" s="22"/>
       <c r="O76" s="22"/>
       <c r="P76" s="10" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="Q76" s="23">
         <v>11014</v>
@@ -3098,7 +3101,7 @@
     </row>
     <row r="77" spans="1:28" ht="15.75">
       <c r="A77" s="10" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="B77" s="21">
         <v>25390</v>
@@ -3133,7 +3136,7 @@
       <c r="N77" s="22"/>
       <c r="O77" s="22"/>
       <c r="P77" s="10" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="Q77" s="23">
         <v>10966</v>
@@ -3174,7 +3177,7 @@
     </row>
     <row r="78" spans="1:28" ht="15.75">
       <c r="A78" s="10" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="B78" s="21">
         <v>24307</v>
@@ -3209,7 +3212,7 @@
       <c r="N78" s="22"/>
       <c r="O78" s="22"/>
       <c r="P78" s="10" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="Q78" s="23">
         <v>9531</v>
@@ -3250,7 +3253,7 @@
     </row>
     <row r="79" spans="1:28" ht="15.75">
       <c r="A79" s="10" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="B79" s="21">
         <v>20421</v>
@@ -3285,7 +3288,7 @@
       <c r="N79" s="22"/>
       <c r="O79" s="22"/>
       <c r="P79" s="10" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="Q79" s="23">
         <v>8055</v>
@@ -3324,7 +3327,7 @@
     </row>
     <row r="80" spans="1:28" ht="15.75">
       <c r="A80" s="10" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="B80" s="21">
         <v>17537</v>
@@ -3359,7 +3362,7 @@
       <c r="N80" s="22"/>
       <c r="O80" s="22"/>
       <c r="P80" s="10" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="Q80" s="23">
         <v>8939</v>
@@ -3398,7 +3401,7 @@
     </row>
     <row r="81" spans="1:40" ht="15.75">
       <c r="A81" s="10" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="B81" s="21">
         <v>19874</v>
@@ -3433,7 +3436,7 @@
       <c r="N81" s="22"/>
       <c r="O81" s="22"/>
       <c r="P81" s="11" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="Q81" s="23">
         <v>7346</v>
@@ -3472,7 +3475,7 @@
     </row>
     <row r="82" spans="1:40" ht="15.75">
       <c r="A82" s="11" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="B82" s="41">
         <v>15791</v>
@@ -3513,7 +3516,7 @@
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
@@ -3528,7 +3531,7 @@
       <c r="R84" s="6"/>
       <c r="S84" s="6"/>
       <c r="T84" s="6" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="U84" s="6"/>
       <c r="V84" s="6"/>
@@ -3594,35 +3597,35 @@
     <row r="86" spans="1:40">
       <c r="A86" s="10"/>
       <c r="B86" s="10" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H86" s="49"/>
       <c r="K86" s="7"/>
       <c r="L86" s="50" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="P86" s="10"/>
       <c r="Q86" s="10"/>
       <c r="S86" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="W86" s="10"/>
       <c r="X86" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="AC86" s="10"/>
       <c r="AD86" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="AI86" s="10"/>
       <c r="AJ86" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="AN86" s="15"/>
     </row>
@@ -3631,115 +3634,115 @@
         <v>58</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C87" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D87" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F87" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="H87" s="51" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="K87" s="14" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="L87" s="14" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="P87" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q87" s="10"/>
       <c r="R87" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="T87" s="10"/>
       <c r="U87" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="W87" s="10"/>
       <c r="X87" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="Z87" s="10"/>
       <c r="AA87" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="AC87" s="10"/>
       <c r="AD87" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="AF87" s="10"/>
       <c r="AG87" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="AI87" s="10"/>
       <c r="AJ87" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="AL87" s="10"/>
       <c r="AM87" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="AN87" s="15"/>
     </row>
     <row r="88" spans="1:40">
       <c r="A88" s="11"/>
       <c r="B88" s="18" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="H88" s="52"/>
       <c r="I88" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J88" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K88" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L88" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
       <c r="P88" s="11"/>
       <c r="Q88" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R88" s="19" t="s">
         <v>57</v>
@@ -3748,7 +3751,7 @@
         <v>58</v>
       </c>
       <c r="T88" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="U88" s="19" t="s">
         <v>57</v>
@@ -3757,7 +3760,7 @@
         <v>58</v>
       </c>
       <c r="W88" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="X88" s="19" t="s">
         <v>57</v>
@@ -3766,7 +3769,7 @@
         <v>58</v>
       </c>
       <c r="Z88" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AA88" s="19" t="s">
         <v>57</v>
@@ -3775,7 +3778,7 @@
         <v>58</v>
       </c>
       <c r="AC88" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AD88" s="19" t="s">
         <v>57</v>
@@ -3784,7 +3787,7 @@
         <v>58</v>
       </c>
       <c r="AF88" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AG88" s="19" t="s">
         <v>57</v>
@@ -3793,7 +3796,7 @@
         <v>58</v>
       </c>
       <c r="AI88" s="18" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="AJ88" s="19" t="s">
         <v>57</v>
@@ -3802,7 +3805,7 @@
         <v>58</v>
       </c>
       <c r="AL88" s="18" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="AM88" s="19" t="s">
         <v>57</v>
@@ -3813,7 +3816,7 @@
     </row>
     <row r="89" spans="1:40" ht="15.75">
       <c r="A89" s="10" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B89" s="21">
         <v>1894</v>
@@ -3851,7 +3854,7 @@
       <c r="M89" s="57"/>
       <c r="N89" s="58"/>
       <c r="P89" s="10" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="Q89" s="25">
         <v>3.8570000000000002</v>
@@ -3928,7 +3931,7 @@
     </row>
     <row r="90" spans="1:40" ht="15.75">
       <c r="A90" s="10" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="B90" s="21">
         <v>1941</v>
@@ -3966,7 +3969,7 @@
       <c r="M90" s="57"/>
       <c r="N90" s="58"/>
       <c r="P90" s="10" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="Q90" s="25">
         <v>4.1280000000000001</v>
@@ -4043,7 +4046,7 @@
     </row>
     <row r="91" spans="1:40" ht="15.75">
       <c r="A91" s="10" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B91" s="21">
         <v>1894</v>
@@ -4081,7 +4084,7 @@
       <c r="M91" s="57"/>
       <c r="N91" s="58"/>
       <c r="P91" s="10" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="Q91" s="25">
         <v>4.9669999999999996</v>
@@ -4158,7 +4161,7 @@
     </row>
     <row r="92" spans="1:40" ht="15.75">
       <c r="A92" s="10" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B92" s="21">
         <v>1890</v>
@@ -4196,7 +4199,7 @@
       <c r="M92" s="57"/>
       <c r="N92" s="58"/>
       <c r="P92" s="10" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="Q92" s="25">
         <v>5.5949999999999998</v>
@@ -4273,7 +4276,7 @@
     </row>
     <row r="93" spans="1:40" ht="15.75">
       <c r="A93" s="10" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="B93" s="21">
         <v>1694</v>
@@ -4311,7 +4314,7 @@
       <c r="M93" s="57"/>
       <c r="N93" s="58"/>
       <c r="P93" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="Q93" s="25">
         <v>5.3390000000000004</v>
@@ -4388,7 +4391,7 @@
     </row>
     <row r="94" spans="1:40" ht="15.75">
       <c r="A94" s="10" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="B94" s="21">
         <v>2133</v>
@@ -4426,7 +4429,7 @@
       <c r="M94" s="57"/>
       <c r="N94" s="58"/>
       <c r="P94" s="10" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="Q94" s="25">
         <v>3.863</v>
@@ -4503,7 +4506,7 @@
     </row>
     <row r="95" spans="1:40" ht="15.75">
       <c r="A95" s="10" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="B95" s="21">
         <v>3223</v>
@@ -4541,7 +4544,7 @@
       <c r="M95" s="57"/>
       <c r="N95" s="58"/>
       <c r="P95" s="10" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="Q95" s="25">
         <v>4.4269999999999996</v>
@@ -4618,7 +4621,7 @@
     </row>
     <row r="96" spans="1:40" ht="15.75">
       <c r="A96" s="10" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="B96" s="21">
         <v>3145</v>
@@ -4656,7 +4659,7 @@
       <c r="M96" s="57"/>
       <c r="N96" s="58"/>
       <c r="P96" s="10" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="Q96" s="25">
         <v>4.7759999999999998</v>
@@ -4733,7 +4736,7 @@
     </row>
     <row r="97" spans="1:40" ht="15.75">
       <c r="A97" s="10" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="B97" s="21">
         <v>4526</v>
@@ -4771,7 +4774,7 @@
       <c r="M97" s="57"/>
       <c r="N97" s="58"/>
       <c r="P97" s="10" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="Q97" s="25">
         <v>3.855</v>
@@ -4848,7 +4851,7 @@
     </row>
     <row r="98" spans="1:40" ht="15.75">
       <c r="A98" s="10" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="B98" s="21">
         <v>4655</v>
@@ -4886,7 +4889,7 @@
       <c r="M98" s="57"/>
       <c r="N98" s="58"/>
       <c r="P98" s="10" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="Q98" s="25">
         <v>3.7589999999999999</v>
@@ -4963,7 +4966,7 @@
     </row>
     <row r="99" spans="1:40" ht="15.75">
       <c r="A99" s="10" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="B99" s="21">
         <v>5456</v>
@@ -5001,7 +5004,7 @@
       <c r="M99" s="57"/>
       <c r="N99" s="58"/>
       <c r="P99" s="10" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="Q99" s="25">
         <v>3.7589999999999999</v>
@@ -5078,7 +5081,7 @@
     </row>
     <row r="100" spans="1:40" ht="15.75">
       <c r="A100" s="10" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="B100" s="21">
         <v>5015</v>
@@ -5116,7 +5119,7 @@
       <c r="M100" s="57"/>
       <c r="N100" s="58"/>
       <c r="P100" s="11" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="Q100" s="25">
         <v>3.7589999999999999</v>
@@ -5193,7 +5196,7 @@
     </row>
     <row r="101" spans="1:40" ht="15.75">
       <c r="A101" s="10" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="B101" s="21">
         <v>6036</v>
@@ -5231,7 +5234,7 @@
       <c r="M101" s="57"/>
       <c r="N101" s="58"/>
       <c r="P101" s="10" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="Q101" s="25">
         <v>5.3010000000000002</v>
@@ -5279,21 +5282,21 @@
         <v>10</v>
       </c>
       <c r="AF101" s="53" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG101" s="30"/>
       <c r="AH101" s="24">
         <v>0</v>
       </c>
       <c r="AI101" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ101" s="30"/>
       <c r="AK101" s="24">
         <v>0</v>
       </c>
       <c r="AL101" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM101" s="30"/>
       <c r="AN101" s="24">
@@ -5302,7 +5305,7 @@
     </row>
     <row r="102" spans="1:40" ht="15.75">
       <c r="A102" s="10" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="B102" s="21">
         <v>6429</v>
@@ -5340,7 +5343,7 @@
       <c r="M102" s="57"/>
       <c r="N102" s="58"/>
       <c r="P102" s="10" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="Q102" s="25">
         <v>5.3010000000000002</v>
@@ -5388,21 +5391,21 @@
         <v>15</v>
       </c>
       <c r="AF102" s="53" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG102" s="30"/>
       <c r="AH102" s="24">
         <v>0</v>
       </c>
       <c r="AI102" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ102" s="30"/>
       <c r="AK102" s="24">
         <v>0</v>
       </c>
       <c r="AL102" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM102" s="30"/>
       <c r="AN102" s="24">
@@ -5449,7 +5452,7 @@
       <c r="M103" s="57"/>
       <c r="N103" s="58"/>
       <c r="P103" s="10" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="Q103" s="25">
         <v>4.6520000000000001</v>
@@ -5497,21 +5500,21 @@
         <v>10</v>
       </c>
       <c r="AF103" s="53" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG103" s="30"/>
       <c r="AH103" s="24">
         <v>0</v>
       </c>
       <c r="AI103" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ103" s="30"/>
       <c r="AK103" s="24">
         <v>0</v>
       </c>
       <c r="AL103" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM103" s="30"/>
       <c r="AN103" s="24">
@@ -5520,7 +5523,7 @@
     </row>
     <row r="104" spans="1:40" ht="15.75">
       <c r="A104" s="10" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="B104" s="21">
         <v>8222</v>
@@ -5558,7 +5561,7 @@
       <c r="M104" s="57"/>
       <c r="N104" s="58"/>
       <c r="P104" s="10" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="Q104" s="25">
         <v>5.6779999999999999</v>
@@ -5606,21 +5609,21 @@
         <v>10</v>
       </c>
       <c r="AF104" s="53" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG104" s="30"/>
       <c r="AH104" s="24">
         <v>0</v>
       </c>
       <c r="AI104" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ104" s="30"/>
       <c r="AK104" s="24">
         <v>0</v>
       </c>
       <c r="AL104" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM104" s="30"/>
       <c r="AN104" s="24">
@@ -5629,7 +5632,7 @@
     </row>
     <row r="105" spans="1:40" ht="15.75">
       <c r="A105" s="10" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="B105" s="21">
         <v>5696</v>
@@ -5667,7 +5670,7 @@
       <c r="M105" s="57"/>
       <c r="N105" s="58"/>
       <c r="P105" s="10" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="Q105" s="25">
         <v>6.0309999999999997</v>
@@ -5715,21 +5718,21 @@
         <v>15</v>
       </c>
       <c r="AF105" s="53" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG105" s="30"/>
       <c r="AH105" s="24">
         <v>0</v>
       </c>
       <c r="AI105" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ105" s="30"/>
       <c r="AK105" s="24">
         <v>0</v>
       </c>
       <c r="AL105" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM105" s="30"/>
       <c r="AN105" s="24">
@@ -5738,7 +5741,7 @@
     </row>
     <row r="106" spans="1:40" ht="15.75">
       <c r="A106" s="10" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="B106" s="21">
         <v>5531</v>
@@ -5776,7 +5779,7 @@
       <c r="M106" s="57"/>
       <c r="N106" s="58"/>
       <c r="P106" s="10" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="Q106" s="25">
         <v>3.85</v>
@@ -5824,21 +5827,21 @@
         <v>15</v>
       </c>
       <c r="AF106" s="53" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG106" s="30"/>
       <c r="AH106" s="24">
         <v>0</v>
       </c>
       <c r="AI106" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ106" s="30"/>
       <c r="AK106" s="24">
         <v>0</v>
       </c>
       <c r="AL106" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM106" s="30"/>
       <c r="AN106" s="24">
@@ -5847,7 +5850,7 @@
     </row>
     <row r="107" spans="1:40" ht="15.75">
       <c r="A107" s="10" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="B107" s="21">
         <v>4689</v>
@@ -5885,7 +5888,7 @@
       <c r="M107" s="57"/>
       <c r="N107" s="58"/>
       <c r="P107" s="10" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="Q107" s="25">
         <v>3.4550000000000001</v>
@@ -5933,21 +5936,21 @@
         <v>8</v>
       </c>
       <c r="AF107" s="53" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG107" s="30"/>
       <c r="AH107" s="24">
         <v>0</v>
       </c>
       <c r="AI107" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ107" s="30"/>
       <c r="AK107" s="24">
         <v>0</v>
       </c>
       <c r="AL107" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM107" s="30"/>
       <c r="AN107" s="24">
@@ -5956,7 +5959,7 @@
     </row>
     <row r="108" spans="1:40" ht="15.75">
       <c r="A108" s="10" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="B108" s="21">
         <v>4855</v>
@@ -5994,7 +5997,7 @@
       <c r="M108" s="57"/>
       <c r="N108" s="58"/>
       <c r="P108" s="11" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
       <c r="Q108" s="25">
         <v>4.4279999999999999</v>
@@ -6042,21 +6045,21 @@
         <v>15</v>
       </c>
       <c r="AF108" s="61" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AG108" s="38"/>
       <c r="AH108" s="43">
         <v>0</v>
       </c>
       <c r="AI108" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AJ108" s="30"/>
       <c r="AK108" s="24">
         <v>0</v>
       </c>
       <c r="AL108" s="59" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="AM108" s="30"/>
       <c r="AN108" s="24">
@@ -6065,7 +6068,7 @@
     </row>
     <row r="109" spans="1:40" ht="15.75">
       <c r="A109" s="10" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="B109" s="21">
         <v>3918</v>
@@ -6105,7 +6108,7 @@
     </row>
     <row r="110" spans="1:40" ht="15.75">
       <c r="A110" s="10" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="B110" s="21">
         <v>3823</v>
@@ -6145,7 +6148,7 @@
     </row>
     <row r="111" spans="1:40" ht="15.75">
       <c r="A111" s="10" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="B111" s="21">
         <v>3748</v>
@@ -6185,7 +6188,7 @@
     </row>
     <row r="112" spans="1:40" ht="15.75">
       <c r="A112" s="11" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="B112" s="41">
         <v>3880</v>
@@ -6226,7 +6229,7 @@
     <row r="115" spans="1:12">
       <c r="A115" s="5"/>
       <c r="B115" s="5" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
@@ -6256,16 +6259,16 @@
     <row r="117" spans="1:12">
       <c r="A117" s="10"/>
       <c r="B117" s="72" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="C117" s="73"/>
       <c r="D117" s="73"/>
       <c r="E117" s="74"/>
       <c r="F117" s="10" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="I117" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J117" s="49"/>
       <c r="K117" s="5"/>
@@ -6273,79 +6276,79 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="10" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="B118" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D118" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="E118" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="F118" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G118" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E118" s="2" t="s">
+      <c r="H118" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F118" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="I118" s="17" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="J118" s="51" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="K118" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L118" s="14" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="11"/>
       <c r="B119" s="18" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="C119" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="E119" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="F119" s="18" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="G119" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="H119" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="I119" s="18" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="J119" s="52"/>
       <c r="K119" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L119" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="15.75">
       <c r="A120" s="64" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="B120" s="23">
         <v>3975.1666666666665</v>
@@ -6383,7 +6386,7 @@
     </row>
     <row r="121" spans="1:12" ht="15.75">
       <c r="A121" s="68" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="B121" s="42">
         <v>5204.083333333333</v>
@@ -6422,7 +6425,7 @@
     <row r="124" spans="1:12">
       <c r="A124" s="5"/>
       <c r="B124" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C124" s="6"/>
       <c r="D124" s="6"/>
@@ -6452,16 +6455,16 @@
     <row r="126" spans="1:12">
       <c r="A126" s="10"/>
       <c r="B126" s="72" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="C126" s="73"/>
       <c r="D126" s="73"/>
       <c r="E126" s="74"/>
       <c r="F126" s="10" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="I126" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J126" s="49"/>
       <c r="K126" s="5"/>
@@ -6469,79 +6472,79 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="10" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="B127" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D127" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="E127" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="F127" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G127" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="H127" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F127" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G127" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="I127" s="17" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="J127" s="51" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="K127" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L127" s="14" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="11"/>
       <c r="B128" s="18" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="E128" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="F128" s="18" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="G128" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="I128" s="18" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="J128" s="52"/>
       <c r="K128" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L128" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="15.75">
       <c r="A129" s="64" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="B129" s="23">
         <v>3061.7916666666665</v>
@@ -6579,7 +6582,7 @@
     </row>
     <row r="130" spans="1:12" ht="15.75">
       <c r="A130" s="68" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="B130" s="42">
         <v>3978.0833333333335</v>

</xml_diff>